<commit_message>
replace 220Ohm R3 from 0402 to 0603
</commit_message>
<xml_diff>
--- a/Bom-DenkyD4.xlsx
+++ b/Bom-DenkyD4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351A01E-17E4-F940-AF40-03EC49AD004A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB3D39-702D-5046-8DA5-645F74CE0FA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9360" yWindow="1560" windowWidth="29040" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>E1</t>
   </si>
   <si>
-    <t>RC0402JR-7D220RL</t>
-  </si>
-  <si>
     <t>RC0402JR-7D330RL</t>
   </si>
   <si>
@@ -280,7 +277,10 @@
     <t>CONUFL001-SMD-T</t>
   </si>
   <si>
-    <t xml:space="preserve">SMD RES 220 Ohm 5%-1/16W-0402 </t>
+    <t>RC0603FR-07220RL</t>
+  </si>
+  <si>
+    <t>SMD RES 220 Ohm 1%-1/16W-0603</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,12 +390,6 @@
       <patternFill patternType="lightUp">
         <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -553,10 +547,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -905,9 +899,9 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -968,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -982,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1">
@@ -990,7 +984,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -1004,13 +998,13 @@
         <v>31</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="19">
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
@@ -1018,13 +1012,13 @@
         <v>22</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -1032,18 +1026,18 @@
         <v>32</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="19">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>9</v>
@@ -1052,12 +1046,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>23</v>
@@ -1066,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
@@ -1080,12 +1074,12 @@
         <v>1</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>5</v>
@@ -1094,12 +1088,12 @@
         <v>2</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>19</v>
@@ -1108,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
@@ -1122,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
@@ -1130,27 +1124,27 @@
         <v>34</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="C19" s="16">
         <v>2</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
@@ -1164,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
@@ -1200,18 +1194,18 @@
         <v>35</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="19">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>68</v>
-      </c>
-      <c r="C23" s="19">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>36</v>
@@ -1220,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
@@ -1228,13 +1222,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="19">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" s="19">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
@@ -1242,13 +1236,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
         <v>74</v>
-      </c>
-      <c r="C26" s="19">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
@@ -1256,13 +1250,13 @@
         <v>21</v>
       </c>
       <c r="B27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="19">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" s="19">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
@@ -1276,12 +1270,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>17</v>
@@ -1295,24 +1289,24 @@
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
         <v>79</v>
-      </c>
-      <c r="C30" s="19">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="18">
         <v>1</v>
@@ -1329,10 +1323,10 @@
         <v>39</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="14.25" customHeight="1">

</xml_diff>